<commit_message>
slight updates to output files
</commit_message>
<xml_diff>
--- a/outgoing/estimates/PRO_est_Steelhead_2014_20200327.xlsx
+++ b/outgoing/estimates/PRO_est_Steelhead_2014_20200327.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/DabomYakimaSthd/outgoing/estimates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_E51AF1DA1C341123FB5EB447DE438136CE7ED28F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE67FE2-EDFA-4C93-A4F3-99F32BEFEC5F}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Escapement" sheetId="1" r:id="rId1"/>
     <sheet name="All Escapement" sheetId="2" r:id="rId2"/>
     <sheet name="Detection" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -231,8 +237,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +284,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -324,7 +338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,9 +370,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,6 +422,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,7 +615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -573,18 +623,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" customWidth="1"/>
+    <col min="5" max="5" width="2.81640625" customWidth="1"/>
+    <col min="6" max="7" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -630,7 +679,7 @@
         <v>1022.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -647,13 +696,13 @@
         <v>37.9</v>
       </c>
       <c r="F3">
-        <v>294.1</v>
+        <v>294.10000000000002</v>
       </c>
       <c r="G3">
         <v>441.8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -676,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -693,13 +742,13 @@
         <v>38.6</v>
       </c>
       <c r="F5">
-        <v>267.9</v>
+        <v>267.89999999999998</v>
       </c>
       <c r="G5">
         <v>421.7</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -728,7 +777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -736,18 +785,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" customWidth="1"/>
+    <col min="5" max="5" width="2.81640625" customWidth="1"/>
+    <col min="6" max="7" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -770,7 +818,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -793,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -801,13 +849,13 @@
         <v>72</v>
       </c>
       <c r="C3">
-        <v>70.6</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="D3">
-        <v>66.9</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="E3">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F3">
         <v>41</v>
@@ -816,7 +864,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -839,7 +887,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -862,15 +910,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="C6">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="D6">
         <v>11.9</v>
@@ -885,7 +933,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -899,7 +947,7 @@
         <v>47.7</v>
       </c>
       <c r="E7">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="F7">
         <v>22.8</v>
@@ -908,7 +956,7 @@
         <v>92.7</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -931,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -954,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -974,10 +1022,10 @@
         <v>58</v>
       </c>
       <c r="G10">
-        <v>129.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>129.69999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1011,19 +1059,19 @@
         <v>2316.4</v>
       </c>
       <c r="D12">
-        <v>2307.7</v>
+        <v>2307.6999999999998</v>
       </c>
       <c r="E12">
-        <v>64.1</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="F12">
-        <v>2191.7</v>
+        <v>2191.6999999999998</v>
       </c>
       <c r="G12">
         <v>2435.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1040,13 +1088,13 @@
         <v>38.6</v>
       </c>
       <c r="F13">
-        <v>267.9</v>
+        <v>267.89999999999998</v>
       </c>
       <c r="G13">
         <v>421.7</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1069,7 +1117,7 @@
         <v>232.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1092,7 +1140,7 @@
         <v>1022.3</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1115,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1132,13 +1180,13 @@
         <v>38.6</v>
       </c>
       <c r="F17">
-        <v>267.9</v>
+        <v>267.89999999999998</v>
       </c>
       <c r="G17">
         <v>421.7</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1161,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1181,10 +1229,10 @@
         <v>18.5</v>
       </c>
       <c r="G19">
-        <v>72.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1207,7 +1255,7 @@
         <v>82.3</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1224,13 +1272,13 @@
         <v>37.9</v>
       </c>
       <c r="F21">
-        <v>294.1</v>
+        <v>294.10000000000002</v>
       </c>
       <c r="G21">
         <v>441.8</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1247,13 +1295,13 @@
         <v>37.9</v>
       </c>
       <c r="F22">
-        <v>294.1</v>
+        <v>294.10000000000002</v>
       </c>
       <c r="G22">
         <v>441.8</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1276,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1305,7 +1353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1313,19 +1361,18 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" customWidth="1"/>
+    <col min="5" max="5" width="5.1796875" customWidth="1"/>
+    <col min="6" max="6" width="2.81640625" customWidth="1"/>
+    <col min="7" max="8" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1385,25 +1432,25 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.686</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="D3">
-        <v>0.701</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="E3">
-        <v>0.787</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="F3">
-        <v>0.171</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="G3">
-        <v>0.352</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="H3">
-        <v>0.973</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.97299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1411,25 +1458,25 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0.821</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="D4">
-        <v>0.857</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="E4">
-        <v>0.947</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="F4">
-        <v>0.147</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="G4">
-        <v>0.535</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1437,25 +1484,25 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.773</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="D5">
-        <v>0.819</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="E5">
-        <v>0.928</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="F5">
-        <v>0.179</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="G5">
-        <v>0.413</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1463,10 +1510,10 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.769</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="D6">
-        <v>0.817</v>
+        <v>0.81699999999999995</v>
       </c>
       <c r="E6">
         <v>0.93</v>
@@ -1481,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1489,25 +1536,25 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>0.822</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="D7">
-        <v>0.857</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="E7">
-        <v>0.951</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="F7">
-        <v>0.148</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="G7">
-        <v>0.518</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1515,13 +1562,13 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0.345</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="D8">
-        <v>0.338</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="E8">
-        <v>0.335</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="F8">
         <v>0.127</v>
@@ -1530,10 +1577,10 @@
         <v>0.113</v>
       </c>
       <c r="H8">
-        <v>0.579</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.57899999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1559,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1567,25 +1614,25 @@
         <v>79</v>
       </c>
       <c r="C10">
-        <v>0.988</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="D10">
-        <v>0.992</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="E10">
         <v>0.997</v>
       </c>
       <c r="F10">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="G10">
-        <v>0.963</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1593,25 +1640,25 @@
         <v>77</v>
       </c>
       <c r="C11">
-        <v>0.963</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="D11">
-        <v>0.967</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="E11">
-        <v>0.977</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="F11">
         <v>0.02</v>
       </c>
       <c r="G11">
-        <v>0.926</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="H11">
         <v>0.996</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1619,25 +1666,25 @@
         <v>201</v>
       </c>
       <c r="C12">
-        <v>0.917</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="D12">
-        <v>0.919</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="E12">
-        <v>0.921</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="F12">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="G12">
-        <v>0.881</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="H12">
-        <v>0.953</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1648,22 +1695,22 @@
         <v>0.99</v>
       </c>
       <c r="D13">
-        <v>0.992</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="E13">
         <v>0.995</v>
       </c>
       <c r="F13">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G13">
-        <v>0.976</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="H13">
         <v>0.999</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1671,25 +1718,25 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>0.904</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="D14">
-        <v>0.931</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="E14">
-        <v>0.972</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="F14">
-        <v>0.088</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="G14">
-        <v>0.724</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1700,10 +1747,10 @@
         <v>0.82</v>
       </c>
       <c r="D15">
-        <v>0.841</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="E15">
-        <v>0.893</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="F15">
         <v>0.111</v>
@@ -1715,7 +1762,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1723,7 +1770,7 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>0.736</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="D16">
         <v>0.75</v>
@@ -1738,10 +1785,10 @@
         <v>0.495</v>
       </c>
       <c r="H16">
-        <v>0.956</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1749,25 +1796,25 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>0.805</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="D17">
-        <v>0.821</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="E17">
-        <v>0.897</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="F17">
-        <v>0.116</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="G17">
         <v>0.59</v>
       </c>
       <c r="H17">
-        <v>0.986</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0.98599999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1775,25 +1822,25 @@
         <v>77</v>
       </c>
       <c r="C18">
-        <v>0.895</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="D18">
-        <v>0.898</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="E18">
-        <v>0.902</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="F18">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G18">
-        <v>0.831</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="H18">
-        <v>0.955</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1801,25 +1848,25 @@
         <v>81</v>
       </c>
       <c r="C19">
-        <v>0.941</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="D19">
-        <v>0.945</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="E19">
-        <v>0.952</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="F19">
-        <v>0.026</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G19">
-        <v>0.891</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="H19">
-        <v>0.988</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1845,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1871,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1897,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1923,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1949,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1975,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2001,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -2027,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -2053,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2079,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -2105,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -2131,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2157,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -2183,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -2209,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -2235,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>69</v>
       </c>

</xml_diff>